<commit_message>
~finished with supplement text
</commit_message>
<xml_diff>
--- a/data/07_md_40_V24-DJH.xlsx
+++ b/data/07_md_40_V24-DJH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danhicks/Google Drive/Coding/*race-science/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D0A49C-7A0C-FE46-BAB7-8FA9B12B6672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE021F3-A4DC-5F49-8EF4-59D02AF2950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="1536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="1536">
   <si>
     <t>topic</t>
   </si>
@@ -4759,6 +4759,11 @@
       <customFilters>
         <customFilter operator="greaterThan" val="0.97"/>
       </customFilters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="n"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
@@ -5090,8 +5095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="F75" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5155,7 +5160,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -5188,7 +5193,7 @@
       </c>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -5221,7 +5226,7 @@
       </c>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -5254,7 +5259,7 @@
       </c>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -5287,7 +5292,7 @@
       </c>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -5320,7 +5325,7 @@
       </c>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -5353,7 +5358,7 @@
       </c>
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -5386,7 +5391,7 @@
       </c>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -5419,7 +5424,7 @@
       </c>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -5452,7 +5457,7 @@
       </c>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -5485,7 +5490,7 @@
       </c>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -5518,7 +5523,7 @@
       </c>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -5551,7 +5556,7 @@
       </c>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -5584,7 +5589,7 @@
       </c>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -5617,7 +5622,7 @@
       </c>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -5684,7 +5689,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -5717,7 +5722,7 @@
       </c>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
@@ -5750,7 +5755,7 @@
       </c>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -5783,7 +5788,7 @@
       </c>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -5816,7 +5821,7 @@
       </c>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -5849,7 +5854,7 @@
       </c>
       <c r="N22"/>
     </row>
-    <row r="23" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -5882,7 +5887,7 @@
       </c>
       <c r="N23"/>
     </row>
-    <row r="24" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -5915,7 +5920,7 @@
       </c>
       <c r="N24"/>
     </row>
-    <row r="25" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
@@ -5948,7 +5953,7 @@
       </c>
       <c r="N25"/>
     </row>
-    <row r="26" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
@@ -5981,7 +5986,7 @@
       </c>
       <c r="N26"/>
     </row>
-    <row r="27" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
@@ -6014,7 +6019,7 @@
       </c>
       <c r="N27"/>
     </row>
-    <row r="28" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
@@ -6047,7 +6052,7 @@
       </c>
       <c r="N28"/>
     </row>
-    <row r="29" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -6080,7 +6085,7 @@
       </c>
       <c r="N29"/>
     </row>
-    <row r="30" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>9</v>
       </c>
@@ -6113,7 +6118,7 @@
       </c>
       <c r="N30"/>
     </row>
-    <row r="31" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>9</v>
       </c>
@@ -6146,7 +6151,7 @@
       </c>
       <c r="N31"/>
     </row>
-    <row r="32" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
@@ -6179,7 +6184,7 @@
       </c>
       <c r="N32"/>
     </row>
-    <row r="33" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
@@ -6212,7 +6217,7 @@
       </c>
       <c r="N33"/>
     </row>
-    <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -6245,7 +6250,7 @@
       </c>
       <c r="N34"/>
     </row>
-    <row r="35" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
@@ -6278,7 +6283,7 @@
       </c>
       <c r="N35"/>
     </row>
-    <row r="36" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
@@ -6311,7 +6316,7 @@
       </c>
       <c r="N36"/>
     </row>
-    <row r="37" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -6379,7 +6384,7 @@
       </c>
       <c r="N38"/>
     </row>
-    <row r="39" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -6412,7 +6417,7 @@
       </c>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
@@ -6445,7 +6450,7 @@
       </c>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>9</v>
       </c>
@@ -6478,7 +6483,7 @@
       </c>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>9</v>
       </c>
@@ -6511,7 +6516,7 @@
       </c>
       <c r="N42"/>
     </row>
-    <row r="43" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>9</v>
       </c>
@@ -6579,7 +6584,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>9</v>
       </c>
@@ -6612,7 +6617,7 @@
       </c>
       <c r="N45"/>
     </row>
-    <row r="46" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
@@ -6680,7 +6685,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>9</v>
       </c>
@@ -6713,7 +6718,7 @@
       </c>
       <c r="N48"/>
     </row>
-    <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
@@ -6746,7 +6751,7 @@
       </c>
       <c r="N49"/>
     </row>
-    <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>9</v>
       </c>
@@ -6779,7 +6784,7 @@
       </c>
       <c r="N50"/>
     </row>
-    <row r="51" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>9</v>
       </c>
@@ -6812,7 +6817,7 @@
       </c>
       <c r="N51"/>
     </row>
-    <row r="52" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>9</v>
       </c>
@@ -6844,7 +6849,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>9</v>
       </c>
@@ -6877,7 +6882,7 @@
       </c>
       <c r="N53"/>
     </row>
-    <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>9</v>
       </c>
@@ -6910,7 +6915,7 @@
       </c>
       <c r="N54"/>
     </row>
-    <row r="55" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
@@ -6943,7 +6948,7 @@
       </c>
       <c r="N55"/>
     </row>
-    <row r="56" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
@@ -7011,7 +7016,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
@@ -7044,7 +7049,7 @@
       </c>
       <c r="N58"/>
     </row>
-    <row r="59" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
@@ -7077,7 +7082,7 @@
       </c>
       <c r="N59"/>
     </row>
-    <row r="60" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>9</v>
       </c>
@@ -7110,7 +7115,7 @@
       </c>
       <c r="N60"/>
     </row>
-    <row r="61" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>9</v>
       </c>
@@ -7143,7 +7148,7 @@
       </c>
       <c r="N61"/>
     </row>
-    <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>9</v>
       </c>
@@ -7176,7 +7181,7 @@
       </c>
       <c r="N62"/>
     </row>
-    <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
@@ -7238,16 +7243,13 @@
         <v>292</v>
       </c>
       <c r="J64" t="s">
-        <v>1515</v>
-      </c>
-      <c r="K64" t="s">
         <v>1514</v>
       </c>
       <c r="N64" t="s">
         <v>1521</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>9</v>
       </c>
@@ -7280,7 +7282,7 @@
       </c>
       <c r="N65"/>
     </row>
-    <row r="66" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>9</v>
       </c>
@@ -7313,7 +7315,7 @@
       </c>
       <c r="N66"/>
     </row>
-    <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
@@ -7346,7 +7348,7 @@
       </c>
       <c r="N67"/>
     </row>
-    <row r="68" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>9</v>
       </c>
@@ -7379,7 +7381,7 @@
       </c>
       <c r="N68"/>
     </row>
-    <row r="69" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>9</v>
       </c>
@@ -7412,7 +7414,7 @@
       </c>
       <c r="N69"/>
     </row>
-    <row r="70" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>9</v>
       </c>
@@ -7445,7 +7447,7 @@
       </c>
       <c r="N70"/>
     </row>
-    <row r="71" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>9</v>
       </c>
@@ -7477,7 +7479,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>9</v>
       </c>
@@ -7510,7 +7512,7 @@
       </c>
       <c r="N72"/>
     </row>
-    <row r="73" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>9</v>
       </c>
@@ -7543,7 +7545,7 @@
       </c>
       <c r="N73"/>
     </row>
-    <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>9</v>
       </c>
@@ -7613,7 +7615,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>9</v>
       </c>
@@ -7646,7 +7648,7 @@
       </c>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>9</v>
       </c>
@@ -7679,7 +7681,7 @@
       </c>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>9</v>
       </c>
@@ -7712,7 +7714,7 @@
       </c>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>9</v>
       </c>
@@ -7745,7 +7747,7 @@
       </c>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>9</v>
       </c>
@@ -7780,7 +7782,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>9</v>
       </c>
@@ -7813,7 +7815,7 @@
       </c>
       <c r="N81"/>
     </row>
-    <row r="82" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>9</v>
       </c>
@@ -7846,7 +7848,7 @@
       </c>
       <c r="N82"/>
     </row>
-    <row r="83" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>9</v>
       </c>
@@ -7879,7 +7881,7 @@
       </c>
       <c r="N83"/>
     </row>
-    <row r="84" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
@@ -7914,7 +7916,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>9</v>
       </c>
@@ -7947,7 +7949,7 @@
       </c>
       <c r="N85"/>
     </row>
-    <row r="86" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>9</v>
       </c>
@@ -8015,7 +8017,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>9</v>
       </c>
@@ -8081,7 +8083,7 @@
       </c>
       <c r="N89"/>
     </row>
-    <row r="90" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>9</v>
       </c>
@@ -8114,7 +8116,7 @@
       </c>
       <c r="N90"/>
     </row>
-    <row r="91" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>9</v>
       </c>
@@ -8180,7 +8182,7 @@
       </c>
       <c r="N92"/>
     </row>
-    <row r="93" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>9</v>
       </c>
@@ -8213,7 +8215,7 @@
       </c>
       <c r="N93"/>
     </row>
-    <row r="94" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -8246,7 +8248,7 @@
       </c>
       <c r="N94"/>
     </row>
-    <row r="95" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>9</v>
       </c>
@@ -8279,7 +8281,7 @@
       </c>
       <c r="N95"/>
     </row>
-    <row r="96" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>9</v>
       </c>
@@ -8312,7 +8314,7 @@
       </c>
       <c r="N96"/>
     </row>
-    <row r="97" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>9</v>
       </c>
@@ -8347,7 +8349,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>9</v>
       </c>
@@ -8380,7 +8382,7 @@
       </c>
       <c r="N98"/>
     </row>
-    <row r="99" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>9</v>
       </c>
@@ -8442,7 +8444,7 @@
         <v>457</v>
       </c>
       <c r="J100" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="M100" t="s">
         <v>1514</v>
@@ -8451,7 +8453,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>9</v>
       </c>
@@ -8484,7 +8486,7 @@
       </c>
       <c r="N101"/>
     </row>
-    <row r="102" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>9</v>
       </c>
@@ -8517,7 +8519,7 @@
       </c>
       <c r="N102"/>
     </row>
-    <row r="103" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>9</v>
       </c>
@@ -8550,7 +8552,7 @@
       </c>
       <c r="N103"/>
     </row>
-    <row r="104" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>9</v>
       </c>
@@ -8583,7 +8585,7 @@
       </c>
       <c r="N104"/>
     </row>
-    <row r="105" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>9</v>
       </c>
@@ -8616,7 +8618,7 @@
       </c>
       <c r="N105"/>
     </row>
-    <row r="106" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>9</v>
       </c>
@@ -8649,7 +8651,7 @@
       </c>
       <c r="N106"/>
     </row>
-    <row r="107" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>9</v>
       </c>
@@ -8717,7 +8719,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>9</v>
       </c>
@@ -8817,14 +8819,11 @@
         <v>504</v>
       </c>
       <c r="J111" t="s">
-        <v>1515</v>
-      </c>
-      <c r="K111" t="s">
         <v>1514</v>
       </c>
       <c r="N111"/>
     </row>
-    <row r="112" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
@@ -8857,7 +8856,7 @@
       </c>
       <c r="N112"/>
     </row>
-    <row r="113" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
@@ -8890,7 +8889,7 @@
       </c>
       <c r="N113"/>
     </row>
-    <row r="114" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>9</v>
       </c>
@@ -8923,7 +8922,7 @@
       </c>
       <c r="N114"/>
     </row>
-    <row r="115" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>9</v>
       </c>
@@ -8956,7 +8955,7 @@
       </c>
       <c r="N115"/>
     </row>
-    <row r="116" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>9</v>
       </c>
@@ -8989,7 +8988,7 @@
       </c>
       <c r="N116"/>
     </row>
-    <row r="117" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>9</v>
       </c>
@@ -9057,7 +9056,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>9</v>
       </c>
@@ -9092,7 +9091,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>9</v>
       </c>
@@ -9125,7 +9124,7 @@
       </c>
       <c r="N120"/>
     </row>
-    <row r="121" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
@@ -9158,7 +9157,7 @@
       </c>
       <c r="N121"/>
     </row>
-    <row r="122" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
@@ -9512,7 +9511,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="134" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>9</v>
       </c>
@@ -14447,7 +14446,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="305" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:9" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>9</v>
       </c>
@@ -15195,7 +15194,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="331" spans="1:9" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:9" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>